<commit_message>
F5A-C and SF5-8 confusion matrices
</commit_message>
<xml_diff>
--- a/figures/confusion matrices.xlsx
+++ b/figures/confusion matrices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nabiki\Desktop\development\schmitz_r-lymphocyte_activation\figures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jriendeau\Documents\GitHub\schmitz_r-lymphocyte_activation\figures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AA0A9A-55F1-4A21-8728-8739036B645C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8CB8C64-632F-4693-9EB7-CA23039830C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -1206,23 +1206,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>297656</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>29766</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>354806</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>39291</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73283179-D470-63C5-600F-3DC1E412A0AA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D5BADDA-98D0-9082-3C9F-814FA4A71BBE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1245,8 +1245,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7362825" y="590550"/>
-          <a:ext cx="2495550" cy="809625"/>
+          <a:off x="7054453" y="422672"/>
+          <a:ext cx="2486025" cy="819150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1267,23 +1267,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>279797</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>148829</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>336947</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>167879</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE06F911-5446-1EAA-AD41-52C836C968A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0EAD6B7-C584-3BFF-BED8-991B14152C53}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1306,8 +1306,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7391400" y="1866900"/>
-          <a:ext cx="2495550" cy="809625"/>
+          <a:off x="7036594" y="1732360"/>
+          <a:ext cx="2486025" cy="816769"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1328,23 +1328,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>279797</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>336947</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>164306</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
+        <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{175C76D0-36A5-2EB2-8598-413124509FA8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B84760F-09CD-604C-725E-3008E9649864}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1367,8 +1367,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7419975" y="3105150"/>
-          <a:ext cx="2495550" cy="809625"/>
+          <a:off x="7036594" y="3309937"/>
+          <a:ext cx="2486025" cy="819150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1394,23 +1394,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14EFB700-91D7-FEB9-D9A5-3D5A7C000C60}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41D9E810-AC39-1C89-DE6F-3E232371900A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1433,7 +1433,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7677150" y="923925"/>
+          <a:off x="7924800" y="1190625"/>
           <a:ext cx="3057525" cy="1009650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1460,23 +1460,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF54B5DC-617B-4DD2-F643-8334E009AAC6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4C1EF5B-9EB6-DCFA-15CA-E033D88EAA15}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1499,7 +1499,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="7658100" y="1323975"/>
+          <a:off x="7924800" y="1552575"/>
           <a:ext cx="3057525" cy="1009650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1526,23 +1526,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1C93F8A-372C-6B55-96AE-6DEB7DDECF97}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C6B78CD-B3FF-8D6E-DEBD-9B0B70F0FDF7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1565,7 +1565,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10972800" y="1933575"/>
+          <a:off x="10696575" y="1514475"/>
           <a:ext cx="5495925" cy="1838325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2769,7 +2769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F196748-038B-428A-A71C-781F5A84D9C5}">
   <dimension ref="B2:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
@@ -3477,8 +3477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B5FDC36-550E-4183-BAFA-124BBCC55894}">
   <dimension ref="A2:K23"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B17"/>
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3543,10 +3543,10 @@
         <v>134</v>
       </c>
       <c r="I5" s="9">
-        <v>676</v>
+        <v>610</v>
       </c>
       <c r="J5" s="7">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="K5" s="6"/>
     </row>
@@ -3557,10 +3557,10 @@
         <v>135</v>
       </c>
       <c r="I6" s="7">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="J6" s="9">
-        <v>1344</v>
+        <v>832</v>
       </c>
       <c r="K6" s="6"/>
     </row>
@@ -3632,10 +3632,10 @@
         <v>134</v>
       </c>
       <c r="I13" s="9">
-        <v>506</v>
+        <v>577</v>
       </c>
       <c r="J13" s="7">
-        <v>262</v>
+        <v>105</v>
       </c>
       <c r="K13" s="6"/>
     </row>
@@ -3652,10 +3652,10 @@
         <v>135</v>
       </c>
       <c r="I14" s="7">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="J14" s="9">
-        <v>1267</v>
+        <v>750</v>
       </c>
       <c r="K14" s="6"/>
     </row>
@@ -3721,10 +3721,10 @@
         <v>134</v>
       </c>
       <c r="I21" s="9">
-        <v>549</v>
+        <v>561</v>
       </c>
       <c r="J21" s="7">
-        <v>219</v>
+        <v>121</v>
       </c>
       <c r="K21" s="6"/>
     </row>
@@ -3738,7 +3738,7 @@
         <v>168</v>
       </c>
       <c r="J22" s="9">
-        <v>1242</v>
+        <v>714</v>
       </c>
       <c r="K22" s="6"/>
     </row>
@@ -3771,8 +3771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3289ACF2-55D6-48B3-8C81-C5AE6EBFCF9E}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A11"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3849,13 +3849,13 @@
         <v>145</v>
       </c>
       <c r="I5" s="9">
-        <v>362</v>
+        <v>590</v>
       </c>
       <c r="J5" s="7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="K5" s="12">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L5" s="6"/>
     </row>
@@ -3866,13 +3866,13 @@
         <v>146</v>
       </c>
       <c r="I6" s="7">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="J6" s="9">
-        <v>368</v>
+        <v>593</v>
       </c>
       <c r="K6" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" s="6"/>
     </row>
@@ -3886,13 +3886,13 @@
         <v>147</v>
       </c>
       <c r="I7" s="12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J7" s="12">
         <v>0</v>
       </c>
       <c r="K7" s="9">
-        <v>1428</v>
+        <v>346</v>
       </c>
       <c r="L7" s="6"/>
     </row>
@@ -3939,8 +3939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FBD06D5-E800-42F7-A73B-99A93393ACC8}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4028,13 +4028,13 @@
         <v>145</v>
       </c>
       <c r="I9" s="9">
-        <v>225</v>
+        <v>365</v>
       </c>
       <c r="J9" s="7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K9" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L9" s="6"/>
     </row>
@@ -4051,7 +4051,7 @@
         <v>2</v>
       </c>
       <c r="J10" s="9">
-        <v>172</v>
+        <v>331</v>
       </c>
       <c r="K10" s="12">
         <v>1</v>
@@ -4068,13 +4068,13 @@
         <v>147</v>
       </c>
       <c r="I11" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11" s="12">
         <v>0</v>
       </c>
       <c r="K11" s="9">
-        <v>985</v>
+        <v>165</v>
       </c>
       <c r="L11" s="6"/>
     </row>
@@ -4110,7 +4110,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{759AF1BA-C6BC-4547-BFAC-3E19A30F4031}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4361,16 +4363,17 @@
         <v>148</v>
       </c>
       <c r="L13" s="13">
-        <v>118</v>
+        <f>B2</f>
+        <v>210</v>
       </c>
       <c r="M13" s="9">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="N13" s="7">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="O13" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="12">
         <v>1</v>
@@ -4388,22 +4391,22 @@
         <v>149</v>
       </c>
       <c r="L14" s="9">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="M14" s="13">
-        <v>222</v>
+        <v>340</v>
       </c>
       <c r="N14" s="7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="O14" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P14" s="12">
         <v>0</v>
       </c>
       <c r="Q14" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R14" s="6"/>
     </row>
@@ -4417,22 +4420,22 @@
         <v>148</v>
       </c>
       <c r="L15" s="7">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M15" s="7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N15" s="13">
-        <v>135</v>
+        <v>223</v>
       </c>
       <c r="O15" s="9">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="P15" s="12">
         <v>0</v>
       </c>
       <c r="Q15" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15" s="6"/>
     </row>
@@ -4447,13 +4450,13 @@
         <v>0</v>
       </c>
       <c r="M16" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N16" s="9">
         <v>29</v>
       </c>
       <c r="O16" s="13">
-        <v>183</v>
+        <v>298</v>
       </c>
       <c r="P16" s="12">
         <v>0</v>
@@ -4485,10 +4488,10 @@
         <v>0</v>
       </c>
       <c r="P17" s="13">
-        <v>421</v>
+        <v>171</v>
       </c>
       <c r="Q17" s="9">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="R17" s="6"/>
     </row>
@@ -4500,10 +4503,10 @@
         <v>149</v>
       </c>
       <c r="L18" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" s="12">
         <v>0</v>
@@ -4512,10 +4515,10 @@
         <v>0</v>
       </c>
       <c r="P18" s="9">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="Q18" s="13">
-        <v>919</v>
+        <v>166</v>
       </c>
       <c r="R18" s="6"/>
     </row>

</xml_diff>